<commit_message>
Changed Truth Table and ALU
</commit_message>
<xml_diff>
--- a/Project/Project_Checkpoint_2/truth_table.xlsx
+++ b/Project/Project_Checkpoint_2/truth_table.xlsx
@@ -165,7 +165,7 @@
     <numFmt numFmtId="164" formatCode="000000"/>
     <numFmt numFmtId="165" formatCode="0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +178,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -258,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -269,12 +275,12 @@
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
@@ -305,6 +311,9 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -317,6 +326,9 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -326,17 +338,17 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -652,19 +664,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="25" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="26" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="27" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="27" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="27" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="27" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="26" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="25" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="25" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="25" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="28" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="28" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="28" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="27" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="28" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="29" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="29" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="29" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="30" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="28" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="27" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="27" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="27" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="30" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="30" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="30" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -683,13 +695,13 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -698,17 +710,17 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -749,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -790,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
@@ -824,10 +836,10 @@
         <v>1</v>
       </c>
       <c r="M4" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
@@ -865,10 +877,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="11">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
@@ -906,10 +918,10 @@
         <v>0</v>
       </c>
       <c r="M6" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
@@ -947,10 +959,10 @@
         <v>0</v>
       </c>
       <c r="M7" s="11">
-        <v>101</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
@@ -988,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="M8" s="11">
-        <v>110</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
@@ -1007,7 +1019,7 @@
       <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="16" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="7">
@@ -1029,10 +1041,10 @@
         <v>1</v>
       </c>
       <c r="M9" s="11">
-        <v>111</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="6" t="s">
         <v>28</v>
       </c>
@@ -1048,7 +1060,7 @@
       <c r="E10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="7">
@@ -1070,10 +1082,10 @@
         <v>1</v>
       </c>
       <c r="M10" s="11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
@@ -1111,366 +1123,366 @@
         <v>0</v>
       </c>
       <c r="M11" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="18">
+        <v>100011</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="20">
+        <v>0</v>
+      </c>
+      <c r="L12" s="20">
+        <v>1</v>
+      </c>
+      <c r="M12" s="20">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="18">
+        <v>101011</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="20">
+        <v>0</v>
+      </c>
+      <c r="L13" s="20">
+        <v>1</v>
+      </c>
+      <c r="M13" s="20">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="18">
+        <v>100</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="20">
+        <v>0</v>
+      </c>
+      <c r="L14" s="20">
+        <v>1</v>
+      </c>
+      <c r="M14" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="18">
+        <v>101</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="20">
+        <v>0</v>
+      </c>
+      <c r="L15" s="20">
+        <v>1</v>
+      </c>
+      <c r="M15" s="20">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="18">
+        <v>10</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="20">
+        <v>0</v>
+      </c>
+      <c r="L16" s="20">
+        <v>1</v>
+      </c>
+      <c r="M16" s="20">
+        <v>17</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="18">
+        <v>11</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="20">
+        <v>0</v>
+      </c>
+      <c r="L17" s="20">
+        <v>1</v>
+      </c>
+      <c r="M17" s="20">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="18">
+        <v>1000</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="20">
+        <v>0</v>
+      </c>
+      <c r="L18" s="20">
+        <v>0</v>
+      </c>
+      <c r="M18" s="20">
+        <v>19</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="18">
+        <v>0</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="18">
         <v>1001</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="17">
-        <v>100011</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="19">
-        <v>0</v>
-      </c>
-      <c r="L12" s="19">
-        <v>1</v>
-      </c>
-      <c r="M12" s="19">
-        <v>1010</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="17">
-        <v>101011</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="19">
-        <v>0</v>
-      </c>
-      <c r="L13" s="19">
-        <v>1</v>
-      </c>
-      <c r="M13" s="19">
-        <v>1011</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="17">
-        <v>100</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="19">
-        <v>0</v>
-      </c>
-      <c r="L14" s="19">
-        <v>1</v>
-      </c>
-      <c r="M14" s="19">
+      <c r="H19" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="20">
+        <v>1</v>
+      </c>
+      <c r="L19" s="20">
+        <v>0</v>
+      </c>
+      <c r="M19" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="18">
+        <v>0</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="18">
         <v>1100</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="17">
-        <v>101</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="19">
-        <v>0</v>
-      </c>
-      <c r="L15" s="19">
-        <v>1</v>
-      </c>
-      <c r="M15" s="19">
-        <v>1101</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="17">
-        <v>10</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="19">
-        <v>0</v>
-      </c>
-      <c r="L16" s="19">
-        <v>1</v>
-      </c>
-      <c r="M16" s="19">
-        <v>1110</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="17">
-        <v>11</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="19">
-        <v>0</v>
-      </c>
-      <c r="L17" s="19">
-        <v>1</v>
-      </c>
-      <c r="M17" s="19">
-        <v>1111</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="17">
-        <v>0</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="17">
-        <v>1000</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="19">
-        <v>0</v>
-      </c>
-      <c r="L18" s="19">
-        <v>0</v>
-      </c>
-      <c r="M18" s="19">
-        <v>10000</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="17">
-        <v>0</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="17">
-        <v>1001</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="19">
-        <v>1</v>
-      </c>
-      <c r="L19" s="19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="19">
-        <v>10001</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="17">
-        <v>0</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="17">
-        <v>1100</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="19">
-        <v>1</v>
-      </c>
-      <c r="L20" s="19">
-        <v>0</v>
-      </c>
-      <c r="M20" s="19">
-        <v>10010</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="H20" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="20">
+        <v>1</v>
+      </c>
+      <c r="L20" s="20">
+        <v>0</v>
+      </c>
+      <c r="M20" s="20">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="22">
-        <v>0</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="23">
-        <v>0</v>
-      </c>
-      <c r="G21" s="22">
+      <c r="B21" s="24">
+        <v>0</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="26">
+        <v>0</v>
+      </c>
+      <c r="G21" s="24">
         <v>100100</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -1482,36 +1494,36 @@
       <c r="J21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="24">
-        <v>1</v>
-      </c>
-      <c r="L21" s="24">
-        <v>0</v>
-      </c>
-      <c r="M21" s="24">
-        <v>10011</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="K21" s="26">
+        <v>1</v>
+      </c>
+      <c r="L21" s="26">
+        <v>0</v>
+      </c>
+      <c r="M21" s="26">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="23">
-        <v>0</v>
-      </c>
-      <c r="G22" s="22">
+      <c r="B22" s="24">
+        <v>0</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="26">
+        <v>0</v>
+      </c>
+      <c r="G22" s="24">
         <v>100101</v>
       </c>
       <c r="H22" s="6" t="s">
@@ -1523,36 +1535,36 @@
       <c r="J22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K22" s="24">
-        <v>1</v>
-      </c>
-      <c r="L22" s="24">
-        <v>0</v>
-      </c>
-      <c r="M22" s="24">
-        <v>10100</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="K22" s="26">
+        <v>1</v>
+      </c>
+      <c r="L22" s="26">
+        <v>0</v>
+      </c>
+      <c r="M22" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="22">
-        <v>0</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="23">
-        <v>0</v>
-      </c>
-      <c r="G23" s="22">
+      <c r="B23" s="24">
+        <v>0</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="26">
+        <v>0</v>
+      </c>
+      <c r="G23" s="24">
         <v>100111</v>
       </c>
       <c r="H23" s="6" t="s">
@@ -1564,36 +1576,36 @@
       <c r="J23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K23" s="24">
-        <v>1</v>
-      </c>
-      <c r="L23" s="24">
-        <v>0</v>
-      </c>
-      <c r="M23" s="24">
-        <v>10101</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="K23" s="26">
+        <v>1</v>
+      </c>
+      <c r="L23" s="26">
+        <v>0</v>
+      </c>
+      <c r="M23" s="26">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="22">
-        <v>0</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="23">
-        <v>0</v>
-      </c>
-      <c r="G24" s="22">
+      <c r="B24" s="24">
+        <v>0</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="26">
+        <v>0</v>
+      </c>
+      <c r="G24" s="24">
         <v>100110</v>
       </c>
       <c r="H24" s="6" t="s">
@@ -1605,105 +1617,105 @@
       <c r="J24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K24" s="24">
-        <v>1</v>
-      </c>
-      <c r="L24" s="24">
-        <v>0</v>
-      </c>
-      <c r="M24" s="24">
-        <v>10111</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="K24" s="26">
+        <v>1</v>
+      </c>
+      <c r="L24" s="26">
+        <v>0</v>
+      </c>
+      <c r="M24" s="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="6"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="22"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="24"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="6"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="22"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="24"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="6"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="22"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="24"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="6"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="22"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="6"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="22"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="6"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="22"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="24"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>